<commit_message>
updated num of hr and tried to not assign for last hr
</commit_message>
<xml_diff>
--- a/timetable.xlsx
+++ b/timetable.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,10 +462,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="60" customWidth="1" min="2" max="2"/>
+    <col width="61" customWidth="1" min="2" max="2"/>
     <col width="37" customWidth="1" min="3" max="3"/>
-    <col width="65" customWidth="1" min="4" max="4"/>
-    <col width="68" customWidth="1" min="5" max="5"/>
+    <col width="57" customWidth="1" min="4" max="4"/>
+    <col width="69" customWidth="1" min="5" max="5"/>
     <col width="37" customWidth="1" min="6" max="6"/>
     <col width="37" customWidth="1" min="7" max="7"/>
   </cols>
@@ -511,7 +511,7 @@
       </c>
       <c r="B2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                </t>
+          <t xml:space="preserve">BLOCKED by                                                 </t>
         </is>
       </c>
       <c r="C2" s="4" t="inlineStr">
@@ -521,12 +521,12 @@
       </c>
       <c r="D2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                     </t>
+          <t xml:space="preserve">BLOCKED by                                             </t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                        </t>
+          <t xml:space="preserve">BLOCKED by                                                         </t>
         </is>
       </c>
       <c r="F2" s="4" t="inlineStr">
@@ -548,7 +548,7 @@
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                </t>
+          <t xml:space="preserve">BLOCKED by                                                 </t>
         </is>
       </c>
       <c r="C3" s="4" t="inlineStr">
@@ -558,12 +558,12 @@
       </c>
       <c r="D3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                     </t>
+          <t xml:space="preserve">BLOCKED by                                             </t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                        </t>
+          <t xml:space="preserve">BLOCKED by                                                         </t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
@@ -585,33 +585,32 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">PSD by NR                                                 </t>
+          <t xml:space="preserve">BLOCKED by                                                 </t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MDC by                             </t>
+          <t xml:space="preserve">BLOCKED by                         </t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
         <is>
-          <t>PSD (Lab - BCA Lab by NR)
- by SME, DR AMRUTHA, MAN, NR, RA, CYN</t>
+          <t xml:space="preserve">BLOCKED by                                             </t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MDC by                                                            </t>
+          <t xml:space="preserve">BLOCKED by                                                         </t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">PSD by NR                          </t>
+          <t xml:space="preserve">BLOCKED by                         </t>
         </is>
       </c>
       <c r="G4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">PSD by NR                          </t>
+          <t xml:space="preserve">BLOCKED by                         </t>
         </is>
       </c>
     </row>
@@ -623,7 +622,7 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">IWT by KR                                                 </t>
+          <t xml:space="preserve">PSD by NR                                                  </t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
@@ -634,23 +633,23 @@
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
-          <t>PSD (Lab - BCA Lab by NR)
- by SME, DR AMRUTHA, MAN, NR, RA, CYN</t>
+          <t>PSD (Lab - BSc Lab by NR)
+ by NR, CYN, KR, SD, SME, FHP</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">language by                                                       </t>
+          <t xml:space="preserve">language by                                                        </t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MATHS by XYZ                       </t>
+          <t xml:space="preserve">PSD by NR                          </t>
         </is>
       </c>
       <c r="G5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MATHS by XYZ                       </t>
+          <t xml:space="preserve">PSD by NR                          </t>
         </is>
       </c>
     </row>
@@ -662,32 +661,33 @@
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">HED by                                                    </t>
+          <t xml:space="preserve">HED by                                                     </t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">PSD by NR                          </t>
+          <t xml:space="preserve">MDC by                             </t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">OOP by SA, CHA                                                 </t>
+          <t>PSD (Lab - BSc Lab by NR)
+ by NR, CYN, KR, SD, SME, FHP</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">OOP by SA, CHA                                                    </t>
+          <t xml:space="preserve">MDC by                                                             </t>
         </is>
       </c>
       <c r="F6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LIBRARY by 1BCAA                   </t>
+          <t xml:space="preserve">MATHS by XYZ                       </t>
         </is>
       </c>
       <c r="G6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LIBRARY by 1BCAA                   </t>
+          <t xml:space="preserve">MATHS by XYZ                       </t>
         </is>
       </c>
     </row>
@@ -699,33 +699,32 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                                  </t>
+          <t xml:space="preserve">IWT by KR                                                  </t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                           </t>
+          <t xml:space="preserve">PSD by NR                          </t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by 
-activity by                                          </t>
+          <t xml:space="preserve">activity by                                            </t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                                          </t>
+          <t xml:space="preserve">OOP by SA, CHA                                                     </t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                           </t>
+          <t xml:space="preserve">LIBRARY by 1BCAA                   </t>
         </is>
       </c>
       <c r="G7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">LIBRARY by 1BCAA                   </t>
         </is>
       </c>
     </row>
@@ -737,34 +736,32 @@
       </c>
       <c r="B8" s="4" t="inlineStr">
         <is>
-          <t>OOP (Lab - BCA Lab by SA, CHA)
- by CHA, RV, KR, NR, SA, SD</t>
+          <t xml:space="preserve">LUNCH by                                                   </t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">OOP (Lab - BCA Lab by SA, CHA)     </t>
+          <t xml:space="preserve">LUNCH by                           </t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">IWT by KR                                                      </t>
+          <t xml:space="preserve">LUNCH by                                               </t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
         <is>
-          <t>IWT (Lab - BCA Lab by KR)
- by DR SARAVANAN KN, MN, KR, BE, TM, RES</t>
+          <t xml:space="preserve">LUNCH by                                                           </t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">LUNCH by                           </t>
         </is>
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
+          <t xml:space="preserve">Free                               </t>
         </is>
       </c>
     </row>
@@ -777,7 +774,7 @@
       <c r="B9" s="4" t="inlineStr">
         <is>
           <t>OOP (Lab - BCA Lab by SA, CHA)
- by CHA, RV, KR, NR, SA, SD</t>
+ by NR, SA, SG, KR, APR, CHA</t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
@@ -787,13 +784,13 @@
       </c>
       <c r="D9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MATHS by XYZ                                                   </t>
+          <t xml:space="preserve">OOP by SA, CHA                                         </t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
         <is>
           <t>IWT (Lab - BCA Lab by KR)
- by DR SARAVANAN KN, MN, KR, BE, TM, RES</t>
+ by LJ, RV, KR, DR SARAVANAN K N, CHA, SD</t>
         </is>
       </c>
       <c r="F9" s="4" t="inlineStr">
@@ -802,6 +799,45 @@
         </is>
       </c>
       <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Hour 9</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>OOP (Lab - BCA Lab by SA, CHA)
+ by NR, SA, SG, KR, APR, CHA</t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OOP (Lab - BCA Lab by SA, CHA)     </t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">IWT by KR                                              </t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t>IWT (Lab - BCA Lab by KR)
+ by LJ, RV, KR, DR SARAVANAN K N, CHA, SD</t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MATHS by XYZ                       </t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">BLOCKED by                         </t>
         </is>
@@ -818,7 +854,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -827,8 +863,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="61" customWidth="1" min="2" max="2"/>
-    <col width="69" customWidth="1" min="3" max="3"/>
+    <col width="74" customWidth="1" min="2" max="2"/>
+    <col width="71" customWidth="1" min="3" max="3"/>
     <col width="37" customWidth="1" min="4" max="4"/>
     <col width="37" customWidth="1" min="5" max="5"/>
     <col width="37" customWidth="1" min="6" max="6"/>
@@ -877,12 +913,12 @@
       <c r="B2" s="4" t="inlineStr">
         <is>
           <t>JAVA (Lab - MCA Lab by SR, MN)
- by LJ, KNS, MN, KR, APR, SR</t>
+ by SR, LJ, RV, MN, APR, DR SARAVANAN K N</t>
         </is>
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">JAVA by SR, MN                                                     </t>
+          <t xml:space="preserve">JAVA by SR, MN                                                       </t>
         </is>
       </c>
       <c r="D2" s="4" t="inlineStr">
@@ -892,7 +928,7 @@
       </c>
       <c r="E2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">INTERNSHIP by 3CM SI               </t>
         </is>
       </c>
       <c r="F2" s="4" t="inlineStr">
@@ -915,12 +951,12 @@
       <c r="B3" s="4" t="inlineStr">
         <is>
           <t>JAVA (Lab - MCA Lab by SR, MN)
- by LJ, KNS, MN, KR, APR, SR</t>
+ by SR, LJ, RV, MN, APR, DR SARAVANAN K N</t>
         </is>
       </c>
       <c r="C3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">JAVA by SR, MN                                                     </t>
+          <t xml:space="preserve">JAVA by SR, MN                                                       </t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
@@ -952,12 +988,12 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                                   </t>
+          <t xml:space="preserve">LUNCH by                                                                </t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                                           </t>
+          <t xml:space="preserve">LUNCH by                                                             </t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -989,18 +1025,18 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">PYTHON by RM                                               </t>
+          <t xml:space="preserve">PYTHON by RM                                                            </t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
         <is>
           <t>PYTHON (Lab - BSc Lab by RM)
- by DR NEWBEGIN, KNS, FHP, RM, RA, SME</t>
+ by NR, RM, SA, SG, KR, DR SARAVANAN K N</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">INTERNSHIP by 3CM SI               </t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -1027,18 +1063,18 @@
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">HED by                                                     </t>
+          <t xml:space="preserve">HED by                                                                  </t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
           <t>PYTHON (Lab - BSc Lab by RM)
- by DR NEWBEGIN, KNS, FHP, RM, RA, SME</t>
+ by NR, RM, SA, SG, KR, DR SARAVANAN K N</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">LIBRARY by 3CM                     </t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -1053,7 +1089,7 @@
       </c>
       <c r="G6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
+          <t xml:space="preserve">Free                               </t>
         </is>
       </c>
     </row>
@@ -1065,12 +1101,12 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LIBRARY by 3CM                                             </t>
+          <t xml:space="preserve">INTERNSHIP by 3CM SI                                                    </t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                               </t>
+          <t xml:space="preserve">INTERNSHIP by 3CM SI                                                 </t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -1102,12 +1138,12 @@
       </c>
       <c r="B8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                 </t>
+          <t xml:space="preserve">BLOCKED by                                                              </t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                         </t>
+          <t xml:space="preserve">BLOCKED by                                                           </t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
@@ -1127,7 +1163,8 @@
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
+          <t xml:space="preserve">BLOCKED by 
+BLOCKED by             </t>
         </is>
       </c>
     </row>
@@ -1139,12 +1176,12 @@
       </c>
       <c r="B9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                 </t>
+          <t xml:space="preserve">BLOCKED by                                                              </t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                         </t>
+          <t xml:space="preserve">BLOCKED by                                                           </t>
         </is>
       </c>
       <c r="D9" s="4" t="inlineStr">
@@ -1163,6 +1200,43 @@
         </is>
       </c>
       <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Hour 9</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                                                              </t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                                                           </t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">BLOCKED by                         </t>
         </is>
@@ -1179,7 +1253,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1188,11 +1262,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="128" customWidth="1" min="2" max="2"/>
+    <col width="80" customWidth="1" min="2" max="2"/>
     <col width="37" customWidth="1" min="3" max="3"/>
-    <col width="84" customWidth="1" min="4" max="4"/>
+    <col width="37" customWidth="1" min="4" max="4"/>
     <col width="37" customWidth="1" min="5" max="5"/>
-    <col width="37" customWidth="1" min="6" max="6"/>
+    <col width="57" customWidth="1" min="6" max="6"/>
     <col width="37" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -1237,7 +1311,7 @@
       </c>
       <c r="B2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                                                                                    </t>
+          <t xml:space="preserve">BLOCKED by                                                                    </t>
         </is>
       </c>
       <c r="C2" s="4" t="inlineStr">
@@ -1247,7 +1321,7 @@
       </c>
       <c r="D2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                                        </t>
+          <t xml:space="preserve">BLOCKED by                         </t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
@@ -1257,7 +1331,7 @@
       </c>
       <c r="F2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
+          <t xml:space="preserve">BLOCKED by                                             </t>
         </is>
       </c>
       <c r="G2" s="4" t="inlineStr">
@@ -1274,7 +1348,7 @@
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                                                                                    </t>
+          <t xml:space="preserve">BLOCKED by                                                                    </t>
         </is>
       </c>
       <c r="C3" s="4" t="inlineStr">
@@ -1284,7 +1358,7 @@
       </c>
       <c r="D3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                                        </t>
+          <t xml:space="preserve">BLOCKED by                         </t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -1294,7 +1368,7 @@
       </c>
       <c r="F3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
+          <t xml:space="preserve">BLOCKED by                                             </t>
         </is>
       </c>
       <c r="G3" s="4" t="inlineStr">
@@ -1311,100 +1385,99 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
+          <t xml:space="preserve">BLOCKED by                                                                    </t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                                             </t>
+        </is>
+      </c>
+      <c r="G4" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Hour 4</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
           <t>WT (Lab - BCA Lab by HU)
 GA (Lab - BCA Lab by CHA)
- by DR NEWBEGIN, HU, SG, SME, FHP, SD
- by DR NEWBEGIN, HU, SG, SME, FHP, SD</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="inlineStr">
+ by SH, SG, MN, KR, HU, FHP</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">WT by HU
 GA by CHA                 </t>
         </is>
       </c>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">WT by HU
-GA by CHA                                                                </t>
-        </is>
-      </c>
-      <c r="E4" s="4" t="inlineStr">
+      <c r="D5" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">WT by HU
 GA by CHA                 </t>
         </is>
       </c>
-      <c r="F4" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Free                               </t>
-        </is>
-      </c>
-      <c r="G4" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Free                               </t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Hour 4</t>
-        </is>
-      </c>
-      <c r="B5" s="4" t="inlineStr">
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">WT by HU
+GA by CHA                 </t>
+        </is>
+      </c>
+      <c r="F5" s="4" t="inlineStr">
+        <is>
+          <t>DA (Lab - BCA Lab by AMR)
+ by RM, AMR, TM, RES, BE, KNS</t>
+        </is>
+      </c>
+      <c r="G5" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                               </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Hour 5</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
         <is>
           <t>WT (Lab - BCA Lab by HU)
 GA (Lab - BCA Lab by CHA)
- by DR NEWBEGIN, HU, SG, SME, FHP, SD
- by DR NEWBEGIN, HU, SG, SME, FHP, SD</t>
-        </is>
-      </c>
-      <c r="C5" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Free                               </t>
-        </is>
-      </c>
-      <c r="D5" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Free                                                                              </t>
-        </is>
-      </c>
-      <c r="E5" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">DA by DR AMRUTHA                   </t>
-        </is>
-      </c>
-      <c r="F5" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Free                               </t>
-        </is>
-      </c>
-      <c r="G5" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Free                               </t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Hour 5</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">DA by DR AMRUTHA                                                                                                              </t>
+ by SH, SG, MN, KR, HU, FHP</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DA by DR AMRUTHA                   </t>
+          <t xml:space="preserve">DA by AMR                          </t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                              </t>
+          <t xml:space="preserve">DA by AMR                          </t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -1414,7 +1487,8 @@
       </c>
       <c r="F6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t>DA (Lab - BCA Lab by AMR)
+ by RM, AMR, TM, RES, BE, KNS</t>
         </is>
       </c>
       <c r="G6" s="4" t="inlineStr">
@@ -1431,27 +1505,27 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                                                                                                      </t>
+          <t xml:space="preserve">DA by AMR                                                                     </t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                           </t>
+          <t xml:space="preserve">Free                               </t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                                                          </t>
+          <t xml:space="preserve">Free                               </t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                           </t>
+          <t xml:space="preserve">Free                               </t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                           </t>
+          <t xml:space="preserve">Free                                                   </t>
         </is>
       </c>
       <c r="G7" s="4" t="inlineStr">
@@ -1468,33 +1542,32 @@
       </c>
       <c r="B8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LIBRARY by 5CME                                                                                                               </t>
+          <t xml:space="preserve">LUNCH by                                                                      </t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">LUNCH by                           </t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
-          <t>DA (Lab - MCA Lab by DR AMRUTHA)
- by DR SARAVANAN KN, VKR, MN, DR AMRUTHA, SR, RES</t>
+          <t xml:space="preserve">LUNCH by                           </t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">LUNCH by                           </t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">LUNCH by                                               </t>
         </is>
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
+          <t xml:space="preserve">Free                               </t>
         </is>
       </c>
     </row>
@@ -1506,7 +1579,7 @@
       </c>
       <c r="B9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                                                                          </t>
+          <t xml:space="preserve">LIBRARY by 5CME                                                               </t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
@@ -1516,8 +1589,7 @@
       </c>
       <c r="D9" s="4" t="inlineStr">
         <is>
-          <t>DA (Lab - MCA Lab by DR AMRUTHA)
- by DR SARAVANAN KN, VKR, MN, DR AMRUTHA, SR, RES</t>
+          <t xml:space="preserve">Free                               </t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
@@ -1527,10 +1599,47 @@
       </c>
       <c r="F9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">Free                                                   </t>
         </is>
       </c>
       <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Hour 9</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                                                                          </t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                               </t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                               </t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                               </t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                                                   </t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">BLOCKED by                         </t>
         </is>
@@ -1547,7 +1656,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1605,7 +1714,7 @@
       </c>
       <c r="B2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">JAVA (Lab - BCA Lab by RES, DR SARAVANAN KN) in 3CS               </t>
+          <t xml:space="preserve">JAVA (Lab - BCA Lab by RES, KNS) in 3CS                           </t>
         </is>
       </c>
       <c r="C2" s="4" t="inlineStr">
@@ -1644,7 +1753,7 @@
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">JAVA (Lab - BCA Lab by RES, DR SARAVANAN KN) in 3CS               </t>
+          <t xml:space="preserve">JAVA (Lab - BCA Lab by RES, KNS) in 3CS                           </t>
         </is>
       </c>
       <c r="C3" s="4" t="inlineStr">
@@ -1683,85 +1792,85 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
+          <t xml:space="preserve">Free                                                              </t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                                    </t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                                      </t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                               </t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                                                                 </t>
+        </is>
+      </c>
+      <c r="G4" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                                                                 </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Hour 4</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
           <t>WT (Lab - BCA Lab by HU) in 5CME
 GA (Lab - BCA Lab by CHA) in 5CME</t>
         </is>
       </c>
-      <c r="C4" s="4" t="inlineStr">
+      <c r="C5" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">Free                                    </t>
         </is>
       </c>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PSD (Lab - BCA Lab by NR) in 1BCA A       </t>
-        </is>
-      </c>
-      <c r="E4" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Free                               </t>
-        </is>
-      </c>
-      <c r="F4" s="4" t="inlineStr">
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                                      </t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                               </t>
+        </is>
+      </c>
+      <c r="F5" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DA (Lab - BCA Lab by AMR) in 5CME                                    </t>
+        </is>
+      </c>
+      <c r="G5" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">Free                                                                 </t>
         </is>
       </c>
-      <c r="G4" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Free                                                                 </t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Hour 4</t>
-        </is>
-      </c>
-      <c r="B5" s="4" t="inlineStr">
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Hour 5</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
         <is>
           <t>WT (Lab - BCA Lab by HU) in 5CME
 GA (Lab - BCA Lab by CHA) in 5CME</t>
         </is>
       </c>
-      <c r="C5" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Free                                    </t>
-        </is>
-      </c>
-      <c r="D5" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PSD (Lab - BCA Lab by NR) in 1BCA A       </t>
-        </is>
-      </c>
-      <c r="E5" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Free                               </t>
-        </is>
-      </c>
-      <c r="F5" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Free                                                                 </t>
-        </is>
-      </c>
-      <c r="G5" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Free                                                                 </t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Hour 5</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MA (Lab - BCA Lab by VKR) in 5BCA A                               </t>
-        </is>
-      </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">MA (Lab - BCA Lab by VKR) in 5BCA A     </t>
@@ -1779,7 +1888,7 @@
       </c>
       <c r="F6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                 </t>
+          <t xml:space="preserve">DA (Lab - BCA Lab by AMR) in 5CME                                    </t>
         </is>
       </c>
       <c r="G6" s="4" t="inlineStr">
@@ -1796,7 +1905,7 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MA (Lab - BCA Lab by VKR) in 5BCA A                               </t>
+          <t xml:space="preserve">Free                                                              </t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -1833,22 +1942,22 @@
       </c>
       <c r="B8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">OOP (Lab - BCA Lab by SA, CHA) in 1BCA A                          </t>
+          <t xml:space="preserve">Free                                                              </t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t>OOP (Lab - BCA Lab by SA, CHA) in 1BCA A</t>
+          <t xml:space="preserve">Free                                    </t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DAS (Lab - BCA Lab by BE) in 1CS          </t>
+          <t xml:space="preserve">Free                                      </t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
         <is>
-          <t>IWT (Lab - BCA Lab by KR) in 1BCA A</t>
+          <t xml:space="preserve">Free                               </t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
@@ -1880,7 +1989,7 @@
       </c>
       <c r="D9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DAS (Lab - BCA Lab by BE) in 1CS          </t>
+          <t xml:space="preserve">PSD (Lab - BCA Lab by APR) in 1BCA B      </t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
@@ -1894,6 +2003,43 @@
         </is>
       </c>
       <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                                                                 </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Hour 9</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OOP (Lab - BCA Lab by SA, CHA) in 1BCA A                          </t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t>OOP (Lab - BCA Lab by SA, CHA) in 1BCA A</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PSD (Lab - BCA Lab by APR) in 1BCA B      </t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t>IWT (Lab - BCA Lab by KR) in 1BCA A</t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                                                                 </t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">Free                                                                 </t>
         </is>
@@ -1910,7 +2056,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1919,12 +2065,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="42" customWidth="1" min="2" max="2"/>
-    <col width="42" customWidth="1" min="3" max="3"/>
+    <col width="55" customWidth="1" min="2" max="2"/>
+    <col width="55" customWidth="1" min="3" max="3"/>
     <col width="45" customWidth="1" min="4" max="4"/>
     <col width="37" customWidth="1" min="5" max="5"/>
-    <col width="89" customWidth="1" min="6" max="6"/>
-    <col width="89" customWidth="1" min="7" max="7"/>
+    <col width="73" customWidth="1" min="6" max="6"/>
+    <col width="73" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1968,12 +2114,12 @@
       </c>
       <c r="B2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">JAVA (Lab - MCA Lab by SR, MN) in 3CM   </t>
+          <t xml:space="preserve">JAVA (Lab - MCA Lab by SR, MN) in 3CM                </t>
         </is>
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                    </t>
+          <t xml:space="preserve">Free                                                 </t>
         </is>
       </c>
       <c r="D2" s="4" t="inlineStr">
@@ -1988,14 +2134,14 @@
       </c>
       <c r="F2" s="4" t="inlineStr">
         <is>
-          <t>BI (Lab - MCA Lab by DR NEWBEGIN) in 5BCA A
-BI (Lab - MCA Lab by DR NEWBEGIN) in 5BCA B</t>
+          <t>BI (Lab - MCA Lab by NEB) in 5BCA A
+BI (Lab - MCA Lab by NEB) in 5BCA B</t>
         </is>
       </c>
       <c r="G2" s="4" t="inlineStr">
         <is>
-          <t>BI (Lab - MCA Lab by DR NEWBEGIN) in 5BCA A
-BI (Lab - MCA Lab by DR NEWBEGIN) in 5BCA B</t>
+          <t>BI (Lab - MCA Lab by NEB) in 5BCA A
+BI (Lab - MCA Lab by NEB) in 5BCA B</t>
         </is>
       </c>
     </row>
@@ -2007,12 +2153,12 @@
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">JAVA (Lab - MCA Lab by SR, MN) in 3CM   </t>
+          <t xml:space="preserve">JAVA (Lab - MCA Lab by SR, MN) in 3CM                </t>
         </is>
       </c>
       <c r="C3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                    </t>
+          <t xml:space="preserve">Free                                                 </t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
@@ -2027,14 +2173,14 @@
       </c>
       <c r="F3" s="4" t="inlineStr">
         <is>
-          <t>BI (Lab - MCA Lab by DR NEWBEGIN) in 5BCA A
-BI (Lab - MCA Lab by DR NEWBEGIN) in 5BCA B</t>
+          <t>BI (Lab - MCA Lab by NEB) in 5BCA A
+BI (Lab - MCA Lab by NEB) in 5BCA B</t>
         </is>
       </c>
       <c r="G3" s="4" t="inlineStr">
         <is>
-          <t>BI (Lab - MCA Lab by DR NEWBEGIN) in 5BCA A
-BI (Lab - MCA Lab by DR NEWBEGIN) in 5BCA B</t>
+          <t>BI (Lab - MCA Lab by NEB) in 5BCA A
+BI (Lab - MCA Lab by NEB) in 5BCA B</t>
         </is>
       </c>
     </row>
@@ -2046,17 +2192,17 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t>OOP (Lab - MCA Lab by KNS, LJ) in 1BCA B</t>
+          <t xml:space="preserve">Free                                                 </t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                    </t>
+          <t xml:space="preserve">Free                                                 </t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">PSD (Lab - MCA Lab by APR) in 1BCA B       </t>
+          <t xml:space="preserve">Free                                       </t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -2066,12 +2212,12 @@
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                                   </t>
+          <t xml:space="preserve">Free                                                                   </t>
         </is>
       </c>
       <c r="G4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                                   </t>
+          <t xml:space="preserve">Free                                                                   </t>
         </is>
       </c>
     </row>
@@ -2083,17 +2229,17 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>OOP (Lab - MCA Lab by KNS, LJ) in 1BCA B</t>
+          <t xml:space="preserve">Free                                                 </t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                    </t>
+          <t xml:space="preserve">Free                                                 </t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">PSD (Lab - MCA Lab by APR) in 1BCA B       </t>
+          <t xml:space="preserve">Free                                       </t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -2103,12 +2249,12 @@
       </c>
       <c r="F5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                                   </t>
+          <t xml:space="preserve">Free                                                                   </t>
         </is>
       </c>
       <c r="G5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                                   </t>
+          <t xml:space="preserve">Free                                                                   </t>
         </is>
       </c>
     </row>
@@ -2120,12 +2266,12 @@
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MA (Lab - MCA Lab by MAN) in 5BCA B     </t>
+          <t xml:space="preserve">MA (Lab - MCA Lab by VKR) in 5BCA A                  </t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MA (Lab - MCA Lab by MAN) in 5BCA B     </t>
+          <t xml:space="preserve">MA (Lab - MCA Lab by MAN) in 5BCA B                  </t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
@@ -2140,12 +2286,12 @@
       </c>
       <c r="F6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                                   </t>
+          <t xml:space="preserve">Free                                                                   </t>
         </is>
       </c>
       <c r="G6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                                   </t>
+          <t xml:space="preserve">Free                                                                   </t>
         </is>
       </c>
     </row>
@@ -2157,12 +2303,12 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MA (Lab - MCA Lab by MAN) in 5BCA B     </t>
+          <t xml:space="preserve">MA (Lab - MCA Lab by VKR) in 5BCA A                  </t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MA (Lab - MCA Lab by MAN) in 5BCA B     </t>
+          <t xml:space="preserve">MA (Lab - MCA Lab by MAN) in 5BCA B                  </t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
@@ -2177,12 +2323,12 @@
       </c>
       <c r="F7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                                   </t>
+          <t xml:space="preserve">Free                                                                   </t>
         </is>
       </c>
       <c r="G7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                                   </t>
+          <t xml:space="preserve">Free                                                                   </t>
         </is>
       </c>
     </row>
@@ -2194,32 +2340,32 @@
       </c>
       <c r="B8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DCF (Lab - MCA Lab by SR, LJ) in 1CS    </t>
+          <t xml:space="preserve">Free                                                 </t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t>OOP (Lab - MCA Lab by KNS, LJ) in 1BCA B</t>
+          <t xml:space="preserve">Free                                                 </t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DA (Lab - MCA Lab by DR AMRUTHA) in 5CME   </t>
+          <t xml:space="preserve">Free                                       </t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
         <is>
-          <t>IWT (Lab - MCA Lab by SG) in 1BCA B</t>
+          <t xml:space="preserve">Free                               </t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                                   </t>
+          <t xml:space="preserve">Free                                                                   </t>
         </is>
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                                   </t>
+          <t xml:space="preserve">Free                                                                   </t>
         </is>
       </c>
     </row>
@@ -2231,17 +2377,17 @@
       </c>
       <c r="B9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DCF (Lab - MCA Lab by SR, LJ) in 1CS    </t>
+          <t>OOP (Lab - MCA Lab by DR SARAVANAN K N, LJ) in 1BCA B</t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
         <is>
-          <t>OOP (Lab - MCA Lab by KNS, LJ) in 1BCA B</t>
+          <t>OOP (Lab - MCA Lab by DR SARAVANAN K N, LJ) in 1BCA B</t>
         </is>
       </c>
       <c r="D9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DA (Lab - MCA Lab by DR AMRUTHA) in 5CME   </t>
+          <t xml:space="preserve">DAS (Lab - MCA Lab by FHP) in 1CM          </t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
@@ -2251,12 +2397,49 @@
       </c>
       <c r="F9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                                   </t>
+          <t xml:space="preserve">Free                                                                   </t>
         </is>
       </c>
       <c r="G9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                                   </t>
+          <t xml:space="preserve">Free                                                                   </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Hour 9</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>OOP (Lab - MCA Lab by DR SARAVANAN K N, LJ) in 1BCA B</t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t>OOP (Lab - MCA Lab by DR SARAVANAN K N, LJ) in 1BCA B</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DAS (Lab - MCA Lab by FHP) in 1CM          </t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t>IWT (Lab - MCA Lab by SG) in 1BCA B</t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                                                                   </t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                                                                   </t>
         </is>
       </c>
     </row>
@@ -2271,7 +2454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2282,7 +2465,7 @@
     <col width="8" customWidth="1" min="1" max="1"/>
     <col width="38" customWidth="1" min="2" max="2"/>
     <col width="37" customWidth="1" min="3" max="3"/>
-    <col width="37" customWidth="1" min="4" max="4"/>
+    <col width="38" customWidth="1" min="4" max="4"/>
     <col width="37" customWidth="1" min="5" max="5"/>
     <col width="37" customWidth="1" min="6" max="6"/>
     <col width="37" customWidth="1" min="7" max="7"/>
@@ -2339,7 +2522,7 @@
       </c>
       <c r="D2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">WAD (Lab - BSc Lab by BE) in 3CS   </t>
+          <t xml:space="preserve">WAD (Lab - BSc Lab by BE) in 3CS    </t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
@@ -2376,7 +2559,7 @@
       </c>
       <c r="D3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">WAD (Lab - BSc Lab by BE) in 3CS   </t>
+          <t xml:space="preserve">WAD (Lab - BSc Lab by BE) in 3CS    </t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -2403,7 +2586,7 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t>DCF (Lab - BSc Lab by SR, MN) in 1CM</t>
+          <t xml:space="preserve">Free                                </t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
@@ -2413,7 +2596,7 @@
       </c>
       <c r="D4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DAS (Lab - BSc Lab by FHP) in 1CM  </t>
+          <t xml:space="preserve">Free                                </t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -2440,7 +2623,7 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>DCF (Lab - BSc Lab by SR, MN) in 1CM</t>
+          <t xml:space="preserve">Free                                </t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
@@ -2450,7 +2633,7 @@
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DAS (Lab - BSc Lab by FHP) in 1CM  </t>
+          <t xml:space="preserve">PSD (Lab - BSc Lab by NR) in 1BCA A </t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -2477,7 +2660,7 @@
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                </t>
+          <t xml:space="preserve">MA (Lab - BSc Lab by MAN) in 5BCA B </t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -2487,7 +2670,7 @@
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">PSD (Lab - BSc Lab by NR) in 1BCA A </t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -2514,17 +2697,17 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
+          <t xml:space="preserve">MA (Lab - BSc Lab by MAN) in 5BCA B </t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                               </t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
           <t xml:space="preserve">Free                                </t>
-        </is>
-      </c>
-      <c r="C7" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Free                               </t>
-        </is>
-      </c>
-      <c r="D7" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Free                               </t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -2556,12 +2739,12 @@
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">WAD (Lab - BSc Lab by TM) in 1CM   </t>
+          <t xml:space="preserve">Free                               </t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">Free                                </t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
@@ -2588,7 +2771,7 @@
       </c>
       <c r="B9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                </t>
+          <t>DCF (Lab - BSc Lab by SR, MN) in 1CM</t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
@@ -2598,12 +2781,12 @@
       </c>
       <c r="D9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t>DCF (Lab - BSc Lab by SR, LJ) in 1CS</t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">DAS (Lab - BSc Lab by BE) in 1CS   </t>
         </is>
       </c>
       <c r="F9" s="4" t="inlineStr">
@@ -2612,6 +2795,43 @@
         </is>
       </c>
       <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                               </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Hour 9</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>DCF (Lab - BSc Lab by SR, MN) in 1CM</t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">WAD (Lab - BSc Lab by TM) in 1CM   </t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t>DCF (Lab - BSc Lab by SR, LJ) in 1CS</t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DAS (Lab - BSc Lab by BE) in 1CS   </t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                               </t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">Free                               </t>
         </is>
@@ -2628,7 +2848,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2637,10 +2857,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="61" customWidth="1" min="2" max="2"/>
-    <col width="37" customWidth="1" min="3" max="3"/>
-    <col width="67" customWidth="1" min="4" max="4"/>
-    <col width="68" customWidth="1" min="5" max="5"/>
+    <col width="88" customWidth="1" min="2" max="2"/>
+    <col width="45" customWidth="1" min="3" max="3"/>
+    <col width="71" customWidth="1" min="4" max="4"/>
+    <col width="58" customWidth="1" min="5" max="5"/>
     <col width="37" customWidth="1" min="6" max="6"/>
     <col width="37" customWidth="1" min="7" max="7"/>
   </cols>
@@ -2686,22 +2906,22 @@
       </c>
       <c r="B2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                 </t>
+          <t xml:space="preserve">BLOCKED by                                                                            </t>
         </is>
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
+          <t xml:space="preserve">BLOCKED by                                 </t>
         </is>
       </c>
       <c r="D2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                       </t>
+          <t xml:space="preserve">BLOCKED by                                                           </t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                        </t>
+          <t xml:space="preserve">BLOCKED by                                              </t>
         </is>
       </c>
       <c r="F2" s="4" t="inlineStr">
@@ -2723,22 +2943,22 @@
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                 </t>
+          <t xml:space="preserve">BLOCKED by                                                                            </t>
         </is>
       </c>
       <c r="C3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
+          <t xml:space="preserve">BLOCKED by                                 </t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                       </t>
+          <t xml:space="preserve">BLOCKED by                                                           </t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                        </t>
+          <t xml:space="preserve">BLOCKED by                                              </t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
@@ -2760,34 +2980,32 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t>OOP (Lab - MCA Lab by KNS, LJ)
- by LJ, KNS, SG, VA, FHP, SD</t>
+          <t xml:space="preserve">BLOCKED by                                                                            </t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MDC by                             </t>
+          <t xml:space="preserve">BLOCKED by                                 </t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
         <is>
-          <t>PSD (Lab - MCA Lab by APR)
- by SME, DR AMRUTHA, MAN, APR, RA, CYN</t>
+          <t xml:space="preserve">BLOCKED by                                                           </t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MDC by                                                            </t>
+          <t xml:space="preserve">BLOCKED by                                              </t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">PSD by APR                         </t>
+          <t xml:space="preserve">BLOCKED by                         </t>
         </is>
       </c>
       <c r="G4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">PSD by APR                         </t>
+          <t xml:space="preserve">BLOCKED by                         </t>
         </is>
       </c>
     </row>
@@ -2799,35 +3017,33 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>OOP (Lab - MCA Lab by KNS, LJ)
- by LJ, KNS, SG, VA, FHP, SD</t>
+          <t xml:space="preserve">PSD by APR                                                                            </t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">MDC by 
-language by                </t>
+language by                        </t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
-          <t>PSD (Lab - MCA Lab by APR)
- by SME, DR AMRUTHA, MAN, APR, RA, CYN</t>
+          <t xml:space="preserve">OOP by DR SARAVANAN K N, LJ                                          </t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">language by                                                       </t>
+          <t xml:space="preserve">language by                                             </t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MATHS by TEMP                      </t>
+          <t xml:space="preserve">PSD by APR                         </t>
         </is>
       </c>
       <c r="G5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MATHS by TEMP                      </t>
+          <t xml:space="preserve">PSD by APR                         </t>
         </is>
       </c>
     </row>
@@ -2839,32 +3055,32 @@
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">HED by                                                     </t>
+          <t xml:space="preserve">HED by                                                                                </t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">PSD by APR                         </t>
+          <t xml:space="preserve">MDC by                                     </t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">OOP by KNS, LJ                                                   </t>
+          <t xml:space="preserve">IWT by SG                                                            </t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">OOP by KNS, LJ                                                    </t>
+          <t xml:space="preserve">MDC by                                                  </t>
         </is>
       </c>
       <c r="F6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LIBRARY by 1BCA B                  </t>
+          <t xml:space="preserve">MATHS by TEMP                      </t>
         </is>
       </c>
       <c r="G6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LIBRARY by 1BCA B                  </t>
+          <t xml:space="preserve">MATHS by TEMP                      </t>
         </is>
       </c>
     </row>
@@ -2876,33 +3092,32 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                                   </t>
+          <t xml:space="preserve">IWT by SG                                                                             </t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                           </t>
+          <t xml:space="preserve">PSD by APR                                 </t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by 
-activity by                                            </t>
+          <t xml:space="preserve">activity by                                                          </t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                                          </t>
+          <t xml:space="preserve">OOP by DR SARAVANAN K N, LJ                             </t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                           </t>
+          <t xml:space="preserve">LIBRARY by 1BCA B                  </t>
         </is>
       </c>
       <c r="G7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">LIBRARY by 1BCA B                  </t>
         </is>
       </c>
     </row>
@@ -2914,33 +3129,32 @@
       </c>
       <c r="B8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">PSD by APR                                                 </t>
+          <t xml:space="preserve">LUNCH by                                                                              </t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">OOP (Lab - MCA Lab by KNS, LJ)     </t>
+          <t xml:space="preserve">LUNCH by                                   </t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">IWT by SG                                                        </t>
+          <t xml:space="preserve">LUNCH by                                                             </t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
         <is>
-          <t>IWT (Lab - MCA Lab by SG)
- by DR SARAVANAN KN, SG, MN, BE, TM, RES</t>
+          <t xml:space="preserve">LUNCH by                                                </t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">LUNCH by                           </t>
         </is>
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
+          <t xml:space="preserve">Free                               </t>
         </is>
       </c>
     </row>
@@ -2952,23 +3166,25 @@
       </c>
       <c r="B9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">IWT by SG                                                  </t>
+          <t>OOP (Lab - MCA Lab by DR SARAVANAN K N, LJ)
+ by LJ, CYN, RV, DR SARAVANAN K N, SD, FHP</t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">OOP (Lab - MCA Lab by KNS, LJ)     </t>
+          <t>OOP (Lab - MCA Lab by DR SARAVANAN K N, LJ)</t>
         </is>
       </c>
       <c r="D9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MATHS by TEMP                                                    </t>
+          <t>PSD (Lab - BCA Lab by APR)
+ by NR, CYN, RV, SG, DR SARAVANAN K N, APR</t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
         <is>
           <t>IWT (Lab - MCA Lab by SG)
- by DR SARAVANAN KN, SG, MN, BE, TM, RES</t>
+ by AMR, VKR, SG, RA, MAN, SME</t>
         </is>
       </c>
       <c r="F9" s="4" t="inlineStr">
@@ -2977,6 +3193,46 @@
         </is>
       </c>
       <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Hour 9</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>OOP (Lab - MCA Lab by DR SARAVANAN K N, LJ)
+ by LJ, CYN, RV, DR SARAVANAN K N, SD, FHP</t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t>OOP (Lab - MCA Lab by DR SARAVANAN K N, LJ)</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t>PSD (Lab - BCA Lab by APR)
+ by NR, CYN, RV, SG, DR SARAVANAN K N, APR</t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t>IWT (Lab - MCA Lab by SG)
+ by AMR, VKR, SG, RA, MAN, SME</t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MATHS by TEMP                      </t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">BLOCKED by                         </t>
         </is>
@@ -2993,7 +3249,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3004,8 +3260,8 @@
     <col width="8" customWidth="1" min="1" max="1"/>
     <col width="37" customWidth="1" min="2" max="2"/>
     <col width="37" customWidth="1" min="3" max="3"/>
-    <col width="62" customWidth="1" min="4" max="4"/>
-    <col width="68" customWidth="1" min="5" max="5"/>
+    <col width="77" customWidth="1" min="4" max="4"/>
+    <col width="58" customWidth="1" min="5" max="5"/>
     <col width="37" customWidth="1" min="6" max="6"/>
     <col width="37" customWidth="1" min="7" max="7"/>
   </cols>
@@ -3062,12 +3318,12 @@
       <c r="D2" s="4" t="inlineStr">
         <is>
           <t>PYTHON (Lab - BCA Lab by TM, VA)
- by LJ, RV, VA, NR, APR, TM</t>
+ by TM, SG, VA, APR, DR SARAVANAN K N, CHA</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">PYTHON by TM, VA                                                  </t>
+          <t xml:space="preserve">PYTHON by TM, VA                                        </t>
         </is>
       </c>
       <c r="F2" s="4" t="inlineStr">
@@ -3100,22 +3356,22 @@
       <c r="D3" s="4" t="inlineStr">
         <is>
           <t>PYTHON (Lab - BCA Lab by TM, VA)
- by LJ, RV, VA, NR, APR, TM</t>
+ by TM, SG, VA, APR, DR SARAVANAN K N, CHA</t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">PYTHON by TM, VA                                                  </t>
+          <t xml:space="preserve">PYTHON by TM, VA                                        </t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">INTERNSHIP by 3BCA A SI            </t>
         </is>
       </c>
       <c r="G3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">INTERNSHIP by 3BCA A SI            </t>
         </is>
       </c>
     </row>
@@ -3137,12 +3393,12 @@
       </c>
       <c r="D4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                                    </t>
+          <t xml:space="preserve">LUNCH by                                                                   </t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                                          </t>
+          <t xml:space="preserve">LUNCH by                                                </t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
@@ -3174,17 +3430,17 @@
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">OS by RV                                                    </t>
+          <t xml:space="preserve">OS by RV                                                                   </t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">language by                                                       </t>
+          <t xml:space="preserve">language by                                             </t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">INTERNSHIP by 3BCA A SI            </t>
         </is>
       </c>
       <c r="G5" s="4" t="inlineStr">
@@ -3211,13 +3467,13 @@
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MA by MAN                                                   </t>
+          <t xml:space="preserve">MA by MAN                                                                  </t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
         <is>
           <t>MA (Lab - BSc Lab by MAN)
- by DR SARAVANAN KN, HU, RM, MAN, TM, BE</t>
+ by AMR, RV, MAN, SD, SME, FHP</t>
         </is>
       </c>
       <c r="F6" s="4" t="inlineStr">
@@ -3227,7 +3483,7 @@
       </c>
       <c r="G6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
+          <t xml:space="preserve">Free                               </t>
         </is>
       </c>
     </row>
@@ -3244,18 +3500,18 @@
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">INTERNSHIP by 3BCA A SI            </t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">activity by                                                 </t>
+          <t xml:space="preserve">activity by                                                                </t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
         <is>
           <t>MA (Lab - BSc Lab by MAN)
- by DR SARAVANAN KN, HU, RM, MAN, TM, BE</t>
+ by AMR, RV, MAN, SD, SME, FHP</t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
@@ -3287,12 +3543,12 @@
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                  </t>
+          <t xml:space="preserve">BLOCKED by                                                                 </t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                        </t>
+          <t xml:space="preserve">BLOCKED by                                              </t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
@@ -3302,7 +3558,8 @@
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
+          <t xml:space="preserve">BLOCKED by 
+BLOCKED by             </t>
         </is>
       </c>
     </row>
@@ -3324,12 +3581,12 @@
       </c>
       <c r="D9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                  </t>
+          <t xml:space="preserve">BLOCKED by                                                                 </t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                        </t>
+          <t xml:space="preserve">BLOCKED by                                              </t>
         </is>
       </c>
       <c r="F9" s="4" t="inlineStr">
@@ -3338,6 +3595,43 @@
         </is>
       </c>
       <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Hour 9</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                                                                 </t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                                              </t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">BLOCKED by                         </t>
         </is>
@@ -3354,7 +3648,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3365,9 +3659,9 @@
     <col width="8" customWidth="1" min="1" max="1"/>
     <col width="37" customWidth="1" min="2" max="2"/>
     <col width="37" customWidth="1" min="3" max="3"/>
-    <col width="73" customWidth="1" min="4" max="4"/>
+    <col width="64" customWidth="1" min="4" max="4"/>
     <col width="37" customWidth="1" min="5" max="5"/>
-    <col width="55" customWidth="1" min="6" max="6"/>
+    <col width="57" customWidth="1" min="6" max="6"/>
     <col width="37" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -3423,7 +3717,7 @@
       <c r="D2" s="4" t="inlineStr">
         <is>
           <t>PYTHON (Lab - MCA Lab by RES, HU)
- by LJ, DR NEWBEGIN, RV, HU, APR, RES</t>
+ by LJ, RES, RV, SD, HU, FHP</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
@@ -3434,12 +3728,12 @@
       <c r="F2" s="4" t="inlineStr">
         <is>
           <t>MA (Lab - BSc Lab by VKR)
- by VKR, HU, RM, SH, TM, BE</t>
+ by AMR, LJ, RV, VKR, RA, CHA</t>
         </is>
       </c>
       <c r="G2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MA by VKR                          </t>
+          <t xml:space="preserve">INTERNSHIP by 3BCA B SI            </t>
         </is>
       </c>
     </row>
@@ -3462,7 +3756,7 @@
       <c r="D3" s="4" t="inlineStr">
         <is>
           <t>PYTHON (Lab - MCA Lab by RES, HU)
- by LJ, DR NEWBEGIN, RV, HU, APR, RES</t>
+ by LJ, RES, RV, SD, HU, FHP</t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -3473,7 +3767,7 @@
       <c r="F3" s="4" t="inlineStr">
         <is>
           <t>MA (Lab - BSc Lab by VKR)
- by VKR, HU, RM, SH, TM, BE</t>
+ by AMR, LJ, RV, VKR, RA, CHA</t>
         </is>
       </c>
       <c r="G3" s="4" t="inlineStr">
@@ -3500,7 +3794,7 @@
       </c>
       <c r="D4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                                               </t>
+          <t xml:space="preserve">LUNCH by                                                      </t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -3510,7 +3804,7 @@
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                             </t>
+          <t xml:space="preserve">LUNCH by                                               </t>
         </is>
       </c>
       <c r="G4" s="4" t="inlineStr">
@@ -3527,7 +3821,7 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">OS by APR                          </t>
+          <t xml:space="preserve">MA by VKR                          </t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
@@ -3537,7 +3831,7 @@
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MA by VKR                                                              </t>
+          <t xml:space="preserve">OS by APR                                                     </t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -3547,7 +3841,7 @@
       </c>
       <c r="F5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                 </t>
+          <t xml:space="preserve">INTERNSHIP by 3BCA B SI                                </t>
         </is>
       </c>
       <c r="G5" s="4" t="inlineStr">
@@ -3569,12 +3863,12 @@
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">OS by APR                          </t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">OS by APR                                                              </t>
+          <t xml:space="preserve">MA by VKR                                                     </t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -3584,12 +3878,12 @@
       </c>
       <c r="F6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                 </t>
+          <t xml:space="preserve">INTERNSHIP by 3BCA B SI                                </t>
         </is>
       </c>
       <c r="G6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
+          <t xml:space="preserve">Free                               </t>
         </is>
       </c>
     </row>
@@ -3601,27 +3895,27 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
+          <t xml:space="preserve">OS by APR                          </t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
           <t xml:space="preserve">LIBRARY by 3 BCA B                 </t>
         </is>
       </c>
-      <c r="C7" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">OS by APR                          </t>
-        </is>
-      </c>
       <c r="D7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">activity by                                                            </t>
+          <t xml:space="preserve">activity by                                                   </t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">INTERNSHIP by 3BCA B SI            </t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                 </t>
+          <t xml:space="preserve">Free                                                   </t>
         </is>
       </c>
       <c r="G7" s="4" t="inlineStr">
@@ -3648,7 +3942,7 @@
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                             </t>
+          <t xml:space="preserve">BLOCKED by                                                    </t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
@@ -3658,12 +3952,13 @@
       </c>
       <c r="F8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                           </t>
+          <t xml:space="preserve">BLOCKED by                                             </t>
         </is>
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
+          <t xml:space="preserve">BLOCKED by 
+BLOCKED by             </t>
         </is>
       </c>
     </row>
@@ -3685,7 +3980,7 @@
       </c>
       <c r="D9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                             </t>
+          <t xml:space="preserve">BLOCKED by                                                    </t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
@@ -3695,10 +3990,47 @@
       </c>
       <c r="F9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                           </t>
+          <t xml:space="preserve">BLOCKED by                                             </t>
         </is>
       </c>
       <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Hour 9</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                                                    </t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                                             </t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">BLOCKED by                         </t>
         </is>
@@ -3715,7 +4047,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3724,12 +4056,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="57" customWidth="1" min="2" max="2"/>
+    <col width="70" customWidth="1" min="2" max="2"/>
     <col width="37" customWidth="1" min="3" max="3"/>
-    <col width="64" customWidth="1" min="4" max="4"/>
+    <col width="57" customWidth="1" min="4" max="4"/>
     <col width="37" customWidth="1" min="5" max="5"/>
-    <col width="98" customWidth="1" min="6" max="6"/>
-    <col width="60" customWidth="1" min="7" max="7"/>
+    <col width="52" customWidth="1" min="6" max="6"/>
+    <col width="52" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3774,39 +4106,37 @@
       <c r="B2" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">GA by VA
-BI by DR NEWBEGIN                             </t>
+BI by NEB                                                  </t>
         </is>
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">GA by VA
-BI by DR NEWBEGIN         </t>
+BI by NEB                 </t>
         </is>
       </c>
       <c r="D2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUL by DR AMRUTHA
+          <t xml:space="preserve">MUL by AMR
 CS by CYN                                   </t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUL by DR AMRUTHA
-CS by CYN        </t>
+          <t xml:space="preserve">MUL by AMR
+CS by CYN               </t>
         </is>
       </c>
       <c r="F2" s="4" t="inlineStr">
         <is>
           <t>GA (Lab - BCA Lab by VA)
-BI (Lab - MCA Lab by DR NEWBEGIN)
- by SH, RM, VA, HU
- by SH, RM, VA, HU</t>
+BI (Lab - MCA Lab by NEB)</t>
         </is>
       </c>
       <c r="G2" s="4" t="inlineStr">
         <is>
           <t>GA (Lab - BCA Lab by VA)
-BI (Lab - MCA Lab by DR NEWBEGIN)</t>
+BI (Lab - MCA Lab by NEB)</t>
         </is>
       </c>
     </row>
@@ -3818,7 +4148,7 @@
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">CN by SME                                              </t>
+          <t xml:space="preserve">CN by SME                                                           </t>
         </is>
       </c>
       <c r="C3" s="4" t="inlineStr">
@@ -3828,7 +4158,7 @@
       </c>
       <c r="D3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MA by VKR                                                     </t>
+          <t xml:space="preserve">MA by VKR                                              </t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -3839,15 +4169,13 @@
       <c r="F3" s="4" t="inlineStr">
         <is>
           <t>GA (Lab - BCA Lab by VA)
-BI (Lab - MCA Lab by DR NEWBEGIN)
- by SH, RM, VA, HU
- by SH, RM, VA, HU</t>
+BI (Lab - MCA Lab by NEB)</t>
         </is>
       </c>
       <c r="G3" s="4" t="inlineStr">
         <is>
           <t>GA (Lab - BCA Lab by VA)
-BI (Lab - MCA Lab by DR NEWBEGIN)</t>
+BI (Lab - MCA Lab by NEB)</t>
         </is>
       </c>
     </row>
@@ -3859,32 +4187,32 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
+          <t xml:space="preserve">LUNCH by                                                            </t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LUNCH by                           </t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
           <t xml:space="preserve">LUNCH by                                               </t>
         </is>
       </c>
-      <c r="C4" s="4" t="inlineStr">
+      <c r="E4" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">LUNCH by                           </t>
         </is>
       </c>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LUNCH by                                                      </t>
-        </is>
-      </c>
-      <c r="E4" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LUNCH by                           </t>
-        </is>
-      </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                                                                        </t>
+          <t xml:space="preserve">LUNCH by                                          </t>
         </is>
       </c>
       <c r="G4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MA by VKR                                                 </t>
+          <t xml:space="preserve">MA by VKR                                         </t>
         </is>
       </c>
     </row>
@@ -3896,36 +4224,36 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUL by DR AMRUTHA
-CS by CYN                            </t>
+          <t xml:space="preserve">MUL by AMR
+CS by CYN                                                </t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUL by DR AMRUTHA
-CS by CYN        </t>
+          <t xml:space="preserve">MUL by AMR
+CS by CYN               </t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">GA by VA
-BI by DR NEWBEGIN                                    </t>
+BI by NEB                                     </t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">GA by VA
-BI by DR NEWBEGIN         </t>
+BI by NEB                 </t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MA by VKR                                                                                       </t>
+          <t xml:space="preserve">MA by VKR                                         </t>
         </is>
       </c>
       <c r="G5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">CN by SME                                                 </t>
+          <t xml:space="preserve">CN by SME                                         </t>
         </is>
       </c>
     </row>
@@ -3937,8 +4265,8 @@
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t>MA (Lab - BCA Lab by VKR)
- by KNS, VKR, CHA, SG, KR, SA</t>
+          <t>MA (Lab - MCA Lab by VKR)
+ by CYN, SA, VKR, VA, DR SARAVANAN K N, SD</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -3949,7 +4277,7 @@
       <c r="D6" s="4" t="inlineStr">
         <is>
           <t>PRJ (Lab - BCA Lab by VA)
- by RV, VA, SME, DR AMRUTHA, RA, CYN</t>
+ by RES, RV, NEB, VA, APR, RA</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -3959,12 +4287,12 @@
       </c>
       <c r="F6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">CN by SME                                                                                       </t>
+          <t xml:space="preserve">CN by SME                                         </t>
         </is>
       </c>
       <c r="G6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                </t>
+          <t xml:space="preserve">Free                                              </t>
         </is>
       </c>
     </row>
@@ -3976,8 +4304,8 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t>MA (Lab - BCA Lab by VKR)
- by KNS, VKR, CHA, SG, KR, SA</t>
+          <t>MA (Lab - MCA Lab by VKR)
+ by CYN, SA, VKR, VA, DR SARAVANAN K N, SD</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -3988,7 +4316,7 @@
       <c r="D7" s="4" t="inlineStr">
         <is>
           <t>PRJ (Lab - BCA Lab by VA)
- by RV, VA, SME, DR AMRUTHA, RA, CYN</t>
+ by RES, RV, NEB, VA, APR, RA</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -3998,12 +4326,12 @@
       </c>
       <c r="F7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LIBRARY by 5 BCA A                                                                              </t>
+          <t xml:space="preserve">LIBRARY by 5 BCA A                                </t>
         </is>
       </c>
       <c r="G7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                </t>
+          <t xml:space="preserve">BLOCKED by                                        </t>
         </is>
       </c>
     </row>
@@ -4015,19 +4343,19 @@
       </c>
       <c r="B8" s="4" t="inlineStr">
         <is>
+          <t xml:space="preserve">BLOCKED by                                                          </t>
+        </is>
+      </c>
+      <c r="C8" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="inlineStr">
+        <is>
           <t xml:space="preserve">BLOCKED by                                             </t>
         </is>
       </c>
-      <c r="C8" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
-        </is>
-      </c>
-      <c r="D8" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">BLOCKED by                                                    </t>
-        </is>
-      </c>
       <c r="E8" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">BLOCKED by                         </t>
@@ -4035,12 +4363,13 @@
       </c>
       <c r="F8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                                                      </t>
+          <t xml:space="preserve">BLOCKED by                                        </t>
         </is>
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                </t>
+          <t xml:space="preserve">BLOCKED by 
+BLOCKED by                            </t>
         </is>
       </c>
     </row>
@@ -4052,19 +4381,19 @@
       </c>
       <c r="B9" s="4" t="inlineStr">
         <is>
+          <t xml:space="preserve">BLOCKED by                                                          </t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="D9" s="4" t="inlineStr">
+        <is>
           <t xml:space="preserve">BLOCKED by                                             </t>
         </is>
       </c>
-      <c r="C9" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
-        </is>
-      </c>
-      <c r="D9" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">BLOCKED by                                                    </t>
-        </is>
-      </c>
       <c r="E9" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">BLOCKED by                         </t>
@@ -4072,12 +4401,49 @@
       </c>
       <c r="F9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                                                      </t>
+          <t xml:space="preserve">BLOCKED by                                        </t>
         </is>
       </c>
       <c r="G9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                </t>
+          <t xml:space="preserve">BLOCKED by                                        </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Hour 9</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                                                          </t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                                             </t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                                        </t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                                        </t>
         </is>
       </c>
     </row>
@@ -4092,7 +4458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4101,12 +4467,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="57" customWidth="1" min="2" max="2"/>
+    <col width="59" customWidth="1" min="2" max="2"/>
     <col width="37" customWidth="1" min="3" max="3"/>
-    <col width="64" customWidth="1" min="4" max="4"/>
+    <col width="51" customWidth="1" min="4" max="4"/>
     <col width="37" customWidth="1" min="5" max="5"/>
-    <col width="90" customWidth="1" min="6" max="6"/>
-    <col width="60" customWidth="1" min="7" max="7"/>
+    <col width="52" customWidth="1" min="6" max="6"/>
+    <col width="52" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4151,39 +4517,37 @@
       <c r="B2" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">GA by VA
-BI by DR NEWBEGIN                             </t>
+BI by NEB                                       </t>
         </is>
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">GA by VA
-BI by DR NEWBEGIN         </t>
+BI by NEB                 </t>
         </is>
       </c>
       <c r="D2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUL by DR AMRUTHA
-CS by CYN                                   </t>
+          <t xml:space="preserve">MUL by AMR
+CS by CYN                             </t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUL by DR AMRUTHA
-CS by CYN        </t>
+          <t xml:space="preserve">MUL by AMR
+CS by CYN               </t>
         </is>
       </c>
       <c r="F2" s="4" t="inlineStr">
         <is>
           <t>GA (Lab - BCA Lab by VA)
-BI (Lab - MCA Lab by DR NEWBEGIN)
- by SH, RM, VA
- by SH, RM, VA</t>
+BI (Lab - MCA Lab by NEB)</t>
         </is>
       </c>
       <c r="G2" s="4" t="inlineStr">
         <is>
           <t>GA (Lab - BCA Lab by VA)
-BI (Lab - MCA Lab by DR NEWBEGIN)</t>
+BI (Lab - MCA Lab by NEB)</t>
         </is>
       </c>
     </row>
@@ -4195,7 +4559,7 @@
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">CN by RA                                               </t>
+          <t xml:space="preserve">CN by RA                                                 </t>
         </is>
       </c>
       <c r="C3" s="4" t="inlineStr">
@@ -4205,7 +4569,7 @@
       </c>
       <c r="D3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MA by MAN                                                     </t>
+          <t xml:space="preserve">MA by MAN                                        </t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -4216,15 +4580,13 @@
       <c r="F3" s="4" t="inlineStr">
         <is>
           <t>GA (Lab - BCA Lab by VA)
-BI (Lab - MCA Lab by DR NEWBEGIN)
- by SH, RM, VA
- by SH, RM, VA</t>
+BI (Lab - MCA Lab by NEB)</t>
         </is>
       </c>
       <c r="G3" s="4" t="inlineStr">
         <is>
           <t>GA (Lab - BCA Lab by VA)
-BI (Lab - MCA Lab by DR NEWBEGIN)</t>
+BI (Lab - MCA Lab by NEB)</t>
         </is>
       </c>
     </row>
@@ -4236,7 +4598,7 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                               </t>
+          <t xml:space="preserve">LUNCH by                                                 </t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
@@ -4246,7 +4608,7 @@
       </c>
       <c r="D4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                                      </t>
+          <t xml:space="preserve">LUNCH by                                         </t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -4256,12 +4618,12 @@
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                                                                </t>
+          <t xml:space="preserve">LUNCH by                                          </t>
         </is>
       </c>
       <c r="G4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MA by MAN                                                 </t>
+          <t xml:space="preserve">MA by MAN                                         </t>
         </is>
       </c>
     </row>
@@ -4273,36 +4635,36 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUL by DR AMRUTHA
-CS by CYN                            </t>
+          <t xml:space="preserve">MUL by AMR
+CS by CYN                                     </t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUL by DR AMRUTHA
-CS by CYN        </t>
+          <t xml:space="preserve">MUL by AMR
+CS by CYN               </t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">GA by VA
-BI by DR NEWBEGIN                                    </t>
+BI by NEB                               </t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">GA by VA
-BI by DR NEWBEGIN         </t>
+BI by NEB                 </t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MA by MAN                                                                               </t>
+          <t xml:space="preserve">MA by MAN                                         </t>
         </is>
       </c>
       <c r="G5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">CN by RA                                                  </t>
+          <t xml:space="preserve">CN by RA                                          </t>
         </is>
       </c>
     </row>
@@ -4314,8 +4676,8 @@
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t>MA (Lab - MCA Lab by MAN)
- by KNS, CHA, SG, KR, SA, MAN</t>
+          <t>MA (Lab - BSc Lab by MAN)
+ by RES, NEB, KNS, RA, MAN, SME</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -4326,7 +4688,7 @@
       <c r="D6" s="4" t="inlineStr">
         <is>
           <t>PRJ (Lab - MCA Lab by SH)
- by RV, SME, DR AMRUTHA, RA, SH, CYN</t>
+ by SH, RM, BE, KNS, HU</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -4336,12 +4698,12 @@
       </c>
       <c r="F6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">CN by RA                                                                                </t>
+          <t xml:space="preserve">CN by RA                                          </t>
         </is>
       </c>
       <c r="G6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                </t>
+          <t xml:space="preserve">Free                                              </t>
         </is>
       </c>
     </row>
@@ -4353,8 +4715,8 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t>MA (Lab - MCA Lab by MAN)
- by KNS, CHA, SG, KR, SA, MAN</t>
+          <t>MA (Lab - BSc Lab by MAN)
+ by RES, NEB, KNS, RA, MAN, SME</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -4365,7 +4727,7 @@
       <c r="D7" s="4" t="inlineStr">
         <is>
           <t>PRJ (Lab - MCA Lab by SH)
- by RV, SME, DR AMRUTHA, RA, SH, CYN</t>
+ by SH, RM, BE, KNS, HU</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -4375,12 +4737,12 @@
       </c>
       <c r="F7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LIBRARY by 5 BCA B                                                                      </t>
+          <t xml:space="preserve">LIBRARY by 5 BCA B                                </t>
         </is>
       </c>
       <c r="G7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                </t>
+          <t xml:space="preserve">BLOCKED by                                        </t>
         </is>
       </c>
     </row>
@@ -4392,7 +4754,7 @@
       </c>
       <c r="B8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                             </t>
+          <t xml:space="preserve">BLOCKED by                                               </t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -4402,7 +4764,7 @@
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                    </t>
+          <t xml:space="preserve">BLOCKED by                                       </t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
@@ -4412,12 +4774,13 @@
       </c>
       <c r="F8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                                              </t>
+          <t xml:space="preserve">BLOCKED by                                        </t>
         </is>
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                </t>
+          <t xml:space="preserve">BLOCKED by 
+BLOCKED by                            </t>
         </is>
       </c>
     </row>
@@ -4429,7 +4792,7 @@
       </c>
       <c r="B9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                             </t>
+          <t xml:space="preserve">BLOCKED by                                               </t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
@@ -4439,7 +4802,7 @@
       </c>
       <c r="D9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                    </t>
+          <t xml:space="preserve">BLOCKED by                                       </t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
@@ -4449,12 +4812,49 @@
       </c>
       <c r="F9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                                              </t>
+          <t xml:space="preserve">BLOCKED by                                        </t>
         </is>
       </c>
       <c r="G9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                </t>
+          <t xml:space="preserve">BLOCKED by                                        </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Hour 9</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                                               </t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                                       </t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                                        </t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                                        </t>
         </is>
       </c>
     </row>
@@ -4469,7 +4869,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4478,10 +4878,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="59" customWidth="1" min="2" max="2"/>
+    <col width="37" customWidth="1" min="2" max="2"/>
     <col width="37" customWidth="1" min="3" max="3"/>
-    <col width="56" customWidth="1" min="4" max="4"/>
-    <col width="37" customWidth="1" min="5" max="5"/>
+    <col width="61" customWidth="1" min="4" max="4"/>
+    <col width="56" customWidth="1" min="5" max="5"/>
     <col width="37" customWidth="1" min="6" max="6"/>
     <col width="37" customWidth="1" min="7" max="7"/>
   </cols>
@@ -4527,7 +4927,7 @@
       </c>
       <c r="B2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                               </t>
+          <t xml:space="preserve">BLOCKED by                         </t>
         </is>
       </c>
       <c r="C2" s="4" t="inlineStr">
@@ -4537,12 +4937,12 @@
       </c>
       <c r="D2" s="4" t="inlineStr">
         <is>
+          <t xml:space="preserve">BLOCKED by                                                 </t>
+        </is>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
           <t xml:space="preserve">BLOCKED by                                            </t>
-        </is>
-      </c>
-      <c r="E2" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
         </is>
       </c>
       <c r="F2" s="4" t="inlineStr">
@@ -4564,7 +4964,7 @@
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                               </t>
+          <t xml:space="preserve">BLOCKED by                         </t>
         </is>
       </c>
       <c r="C3" s="4" t="inlineStr">
@@ -4574,12 +4974,12 @@
       </c>
       <c r="D3" s="4" t="inlineStr">
         <is>
+          <t xml:space="preserve">BLOCKED by                                                 </t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
           <t xml:space="preserve">BLOCKED by                                            </t>
-        </is>
-      </c>
-      <c r="E3" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
@@ -4601,32 +5001,32 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DAS by BE                                                </t>
+          <t xml:space="preserve">BLOCKED by                         </t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MDC by                             </t>
+          <t xml:space="preserve">BLOCKED by                         </t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DCF by SR, LJ                                         </t>
+          <t xml:space="preserve">BLOCKED by                                                 </t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MDC by                             </t>
+          <t xml:space="preserve">BLOCKED by                                            </t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">BLOCKED by                         </t>
         </is>
       </c>
       <c r="G4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">BLOCKED by                         </t>
         </is>
       </c>
     </row>
@@ -4638,7 +5038,7 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LIBRARY by 1CS                                           </t>
+          <t xml:space="preserve">DCF by SR, LJ                      </t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
@@ -4649,17 +5049,17 @@
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                  </t>
+          <t xml:space="preserve">Free                                                       </t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">language by                        </t>
+          <t xml:space="preserve">language by                                           </t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">DCF by SR, LJ                      </t>
         </is>
       </c>
       <c r="G5" s="4" t="inlineStr">
@@ -4676,22 +5076,22 @@
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">HED by                                                   </t>
+          <t xml:space="preserve">HED by                             </t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DCF by LJ                          </t>
+          <t xml:space="preserve">MDC by                             </t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                  </t>
+          <t xml:space="preserve">Free                                                       </t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">MDC by                                                </t>
         </is>
       </c>
       <c r="F6" s="4" t="inlineStr">
@@ -4713,28 +5113,27 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                                 </t>
+          <t xml:space="preserve">DAS by BE                          </t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                           </t>
+          <t xml:space="preserve">DCF by LJ                          </t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by 
-activity by                                 </t>
+          <t xml:space="preserve">activity by                                                </t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                           </t>
+          <t xml:space="preserve">Free                                                  </t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                           </t>
+          <t xml:space="preserve">Free                               </t>
         </is>
       </c>
       <c r="G7" s="4" t="inlineStr">
@@ -4751,34 +5150,32 @@
       </c>
       <c r="B8" s="4" t="inlineStr">
         <is>
-          <t>DCF (Lab - MCA Lab by SR, LJ)
- by LJ, KNS, KR, NR, SR, SD</t>
+          <t xml:space="preserve">LUNCH by                           </t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DAS by BE                          </t>
+          <t xml:space="preserve">LUNCH by                           </t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
-          <t>DAS (Lab - BCA Lab by BE)
- by VKR, RV, RA, CYN, SR, BE</t>
+          <t xml:space="preserve">LUNCH by                                                   </t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DCF by SR, LJ                      </t>
+          <t xml:space="preserve">LUNCH by                                              </t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">LUNCH by                           </t>
         </is>
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
+          <t xml:space="preserve">Free                               </t>
         </is>
       </c>
     </row>
@@ -4790,24 +5187,24 @@
       </c>
       <c r="B9" s="4" t="inlineStr">
         <is>
-          <t>DCF (Lab - MCA Lab by SR, LJ)
- by LJ, KNS, KR, NR, SR, SD</t>
+          <t xml:space="preserve">LIBRARY by 1CS                     </t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">DAS by BE                          </t>
         </is>
       </c>
       <c r="D9" s="4" t="inlineStr">
         <is>
-          <t>DAS (Lab - BCA Lab by BE)
- by VKR, RV, RA, CYN, SR, BE</t>
+          <t>DCF (Lab - BSc Lab by SR, LJ)
+ by SR, LJ, VKR, NEB, SD, SME</t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t>DAS (Lab - BSc Lab by BE)
+ by SR, RM, TM, RES, BE, KNS</t>
         </is>
       </c>
       <c r="F9" s="4" t="inlineStr">
@@ -4816,6 +5213,45 @@
         </is>
       </c>
       <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Hour 9</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                               </t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                               </t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t>DCF (Lab - BSc Lab by SR, LJ)
+ by SR, LJ, VKR, NEB, SD, SME</t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t>DAS (Lab - BSc Lab by BE)
+ by SR, RM, TM, RES, BE, KNS</t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                               </t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">BLOCKED by                         </t>
         </is>
@@ -4832,7 +5268,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4841,9 +5277,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="89" customWidth="1" min="2" max="2"/>
+    <col width="64" customWidth="1" min="2" max="2"/>
     <col width="37" customWidth="1" min="3" max="3"/>
-    <col width="63" customWidth="1" min="4" max="4"/>
+    <col width="57" customWidth="1" min="4" max="4"/>
     <col width="37" customWidth="1" min="5" max="5"/>
     <col width="37" customWidth="1" min="6" max="6"/>
     <col width="37" customWidth="1" min="7" max="7"/>
@@ -4890,29 +5326,29 @@
       </c>
       <c r="B2" s="4" t="inlineStr">
         <is>
-          <t>JAVA (Lab - BCA Lab by RES, DR SARAVANAN KN)
- by KNS, DR SARAVANAN KN, CHA, KR, SA, RES</t>
+          <t>JAVA (Lab - BCA Lab by RES, KNS)
+ by RES, SA, SG, KR, CHA, KNS</t>
         </is>
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">JAVA by RES, DR SARAVANAN KN       </t>
+          <t xml:space="preserve">JAVA by RES, KNS                   </t>
         </is>
       </c>
       <c r="D2" s="4" t="inlineStr">
         <is>
           <t>WAD (Lab - BSc Lab by BE)
- by DR SARAVANAN KN, RV, SH, RA, BE</t>
+ by SH, NEB, KNS, BE, RA, SME</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">INTERNSHIP by 3CS SI               </t>
         </is>
       </c>
       <c r="F2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">JAVA by RES, DR SARAVANAN KN       </t>
+          <t xml:space="preserve">JAVA by RES, KNS                   </t>
         </is>
       </c>
       <c r="G2" s="4" t="inlineStr">
@@ -4929,19 +5365,19 @@
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t>JAVA (Lab - BCA Lab by RES, DR SARAVANAN KN)
- by KNS, DR SARAVANAN KN, CHA, KR, SA, RES</t>
+          <t>JAVA (Lab - BCA Lab by RES, KNS)
+ by RES, SA, SG, KR, CHA, KNS</t>
         </is>
       </c>
       <c r="C3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">JAVA by RES, DR SARAVANAN KN       </t>
+          <t xml:space="preserve">JAVA by RES, KNS                   </t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
         <is>
           <t>WAD (Lab - BSc Lab by BE)
- by DR SARAVANAN KN, RV, SH, RA, BE</t>
+ by SH, NEB, KNS, BE, RA, SME</t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -4968,7 +5404,7 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                                                               </t>
+          <t xml:space="preserve">LUNCH by                                                      </t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
@@ -4978,7 +5414,7 @@
       </c>
       <c r="D4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                                     </t>
+          <t xml:space="preserve">LUNCH by                                               </t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -5005,7 +5441,7 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">WAD by BE                                                                              </t>
+          <t xml:space="preserve">WAD by BE                                                     </t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
@@ -5015,7 +5451,7 @@
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                         </t>
+          <t xml:space="preserve">INTERNSHIP by 3CS SI                                   </t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -5042,17 +5478,17 @@
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">HED by                                                                                 </t>
+          <t xml:space="preserve">HED by                                                        </t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LIBRARY by 3CM                     </t>
+          <t xml:space="preserve">INTERNSHIP by 3CS SI               </t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                         </t>
+          <t xml:space="preserve">Free                                                   </t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -5067,7 +5503,7 @@
       </c>
       <c r="G6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
+          <t xml:space="preserve">Free                               </t>
         </is>
       </c>
     </row>
@@ -5079,17 +5515,17 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                                                                                   </t>
+          <t xml:space="preserve">INTERNSHIP by 3CS SI                                          </t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">LIBRARY by 3CM                     </t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">activity by                                                  </t>
+          <t xml:space="preserve">activity by                                            </t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -5116,7 +5552,7 @@
       </c>
       <c r="B8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                                             </t>
+          <t xml:space="preserve">BLOCKED by                                                    </t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -5126,7 +5562,7 @@
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                   </t>
+          <t xml:space="preserve">BLOCKED by                                             </t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
@@ -5141,7 +5577,8 @@
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
+          <t xml:space="preserve">BLOCKED by 
+BLOCKED by             </t>
         </is>
       </c>
     </row>
@@ -5153,7 +5590,7 @@
       </c>
       <c r="B9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                                             </t>
+          <t xml:space="preserve">BLOCKED by                                                    </t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
@@ -5163,7 +5600,7 @@
       </c>
       <c r="D9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                   </t>
+          <t xml:space="preserve">BLOCKED by                                             </t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
@@ -5177,6 +5614,43 @@
         </is>
       </c>
       <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Hour 9</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                                                    </t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                                             </t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">BLOCKED by                         </t>
         </is>
@@ -5193,7 +5667,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5202,9 +5676,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="68" customWidth="1" min="2" max="2"/>
-    <col width="55" customWidth="1" min="3" max="3"/>
-    <col width="70" customWidth="1" min="4" max="4"/>
+    <col width="62" customWidth="1" min="2" max="2"/>
+    <col width="56" customWidth="1" min="3" max="3"/>
+    <col width="60" customWidth="1" min="4" max="4"/>
     <col width="37" customWidth="1" min="5" max="5"/>
     <col width="37" customWidth="1" min="6" max="6"/>
     <col width="37" customWidth="1" min="7" max="7"/>
@@ -5251,17 +5725,17 @@
       </c>
       <c r="B2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                        </t>
+          <t xml:space="preserve">BLOCKED by                                                  </t>
         </is>
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                           </t>
+          <t xml:space="preserve">BLOCKED by                                            </t>
         </is>
       </c>
       <c r="D2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                          </t>
+          <t xml:space="preserve">BLOCKED by                                                </t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
@@ -5288,17 +5762,17 @@
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                        </t>
+          <t xml:space="preserve">BLOCKED by                                                  </t>
         </is>
       </c>
       <c r="C3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                           </t>
+          <t xml:space="preserve">BLOCKED by                                            </t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                                                          </t>
+          <t xml:space="preserve">BLOCKED by                                                </t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -5325,34 +5799,32 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t>DCF (Lab - BSc Lab by SR, MN)
- by DR NEWBEGIN, MN, SG, FHP, SR, SD</t>
+          <t xml:space="preserve">BLOCKED by                                                  </t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MDC by                                               </t>
+          <t xml:space="preserve">BLOCKED by                                            </t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
         <is>
-          <t>DAS (Lab - BSc Lab by FHP)
- by DR SARAVANAN KN, MN, BE, FHP, TM, RES</t>
+          <t xml:space="preserve">BLOCKED by                                                </t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">MDC by                             </t>
+          <t xml:space="preserve">BLOCKED by                         </t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">BLOCKED by                         </t>
         </is>
       </c>
       <c r="G4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">BLOCKED by                         </t>
         </is>
       </c>
     </row>
@@ -5364,20 +5836,18 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>DCF (Lab - BSc Lab by SR, MN)
- by DR NEWBEGIN, MN, SG, FHP, SR, SD</t>
+          <t xml:space="preserve">WAD by TM                                                   </t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">MDC by 
-language by                                  </t>
+language by                                   </t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
-          <t>DAS (Lab - BSc Lab by FHP)
- by DR SARAVANAN KN, MN, BE, FHP, TM, RES</t>
+          <t xml:space="preserve">DCF by SR, MN                                             </t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -5404,22 +5874,22 @@
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">HED by                                                            </t>
+          <t xml:space="preserve">HED by                                                      </t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DCF by SR, MN                                        </t>
+          <t xml:space="preserve">MDC by                                                </t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DCF by SR, MN                                                       </t>
+          <t xml:space="preserve">WAD by TM                                                 </t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DCF by SR, MN                      </t>
+          <t xml:space="preserve">MDC by                             </t>
         </is>
       </c>
       <c r="F6" s="4" t="inlineStr">
@@ -5441,28 +5911,27 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                                          </t>
+          <t xml:space="preserve">DAS by FHP                                                  </t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                                             </t>
+          <t xml:space="preserve">DCF by SR, MN                                         </t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by 
-activity by                                               </t>
+          <t xml:space="preserve">activity by                                               </t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                           </t>
+          <t xml:space="preserve">DCF by SR, MN                      </t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LUNCH by                           </t>
+          <t xml:space="preserve">Free                               </t>
         </is>
       </c>
       <c r="G7" s="4" t="inlineStr">
@@ -5479,33 +5948,32 @@
       </c>
       <c r="B8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">WAD by TM                                                         </t>
+          <t xml:space="preserve">LUNCH by                                                    </t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t>WAD (Lab - BSc Lab by TM)
- by SG, KR, NR, APR, TM, SD</t>
+          <t xml:space="preserve">LUNCH by                                              </t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">WAD by TM                                                           </t>
+          <t xml:space="preserve">LUNCH by                                                  </t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DAS by FHP                         </t>
+          <t xml:space="preserve">LUNCH by                           </t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">LUNCH by                           </t>
         </is>
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BLOCKED by                         </t>
+          <t xml:space="preserve">Free                               </t>
         </is>
       </c>
     </row>
@@ -5517,23 +5985,25 @@
       </c>
       <c r="B9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DAS by FHP                                                        </t>
+          <t>DCF (Lab - BSc Lab by SR, MN)
+ by SR, AMR, VKR, NEB, MN, SME</t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
         <is>
           <t>WAD (Lab - BSc Lab by TM)
- by SG, KR, NR, APR, TM, SD</t>
+ by NR, TM, CYN, SG, KR, APR</t>
         </is>
       </c>
       <c r="D9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">LIBRARY by 1CM                                                      </t>
+          <t>DAS (Lab - MCA Lab by FHP)
+ by AMR, RES, RA, MAN, KNS, FHP</t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free                               </t>
+          <t xml:space="preserve">DAS by FHP                         </t>
         </is>
       </c>
       <c r="F9" s="4" t="inlineStr">
@@ -5542,6 +6012,46 @@
         </is>
       </c>
       <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BLOCKED by                         </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Hour 9</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>DCF (Lab - BSc Lab by SR, MN)
+ by SR, AMR, VKR, NEB, MN, SME</t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t>WAD (Lab - BSc Lab by TM)
+ by NR, TM, CYN, SG, KR, APR</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t>DAS (Lab - MCA Lab by FHP)
+ by AMR, RES, RA, MAN, KNS, FHP</t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LIBRARY by 1CM                     </t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Free                               </t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">BLOCKED by                         </t>
         </is>

</xml_diff>